<commit_message>
Spreadsheets from meetings added
</commit_message>
<xml_diff>
--- a/Champs Scouting.xlsx
+++ b/Champs Scouting.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adam\Desktop\Scouting2017\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adam Schoenberg\Desktop\Robonauts2018\Scouting2018\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7530" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7530" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RAW" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Scouting!$A$2:$AN$51</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Second Pick Ranking'!$A$1:$AC$68</definedName>
   </definedNames>
-  <calcPr calcId="171027" calcCompleted="0"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -17415,11 +17415,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AN69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="AN68" workbookViewId="0">
       <pane xSplit="1350" ySplit="900" topLeftCell="B3" activePane="bottomRight"/>
+      <selection sqref="A1:AN69"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AN3" sqref="AN3"/>
+      <selection pane="bottomRight" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28221,10 +28222,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AD69"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="AC1" sqref="AC1"/>
+      <selection pane="bottomLeft" activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>